<commit_message>
code update and add comments
</commit_message>
<xml_diff>
--- a/Clinical/ADAM_METADATA.xlsx
+++ b/Clinical/ADAM_METADATA.xlsx
@@ -5,11 +5,11 @@
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\GitHub\SAS\Clinical\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Clinical Portfolio\Clinical\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="120" windowWidth="19005" windowHeight="7590" tabRatio="853" activeTab="2"/>
+    <workbookView xWindow="-15" yWindow="120" windowWidth="19005" windowHeight="7590" tabRatio="853" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="DefineHeader" sheetId="4" r:id="rId1"/>
@@ -24,7 +24,7 @@
     <sheet name="ExternalLinks" sheetId="9" r:id="rId10"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">VariableLevel!$A$1:$P$43</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">VariableLevel!$A$1:$P$62</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
@@ -90,7 +90,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="899" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1025" uniqueCount="357">
   <si>
     <t>STUDYID, USUBJID</t>
   </si>
@@ -344,6 +344,9 @@
     <t>0</t>
   </si>
   <si>
+    <t>Y</t>
+  </si>
+  <si>
     <t>Baseline</t>
   </si>
   <si>
@@ -428,12 +431,21 @@
     <t>ABLFL</t>
   </si>
   <si>
+    <t>Baseline Record Flag</t>
+  </si>
+  <si>
     <t>ADT</t>
   </si>
   <si>
+    <t>Analysis Date</t>
+  </si>
+  <si>
     <t>ADY</t>
   </si>
   <si>
+    <t>Analysis Relative Day</t>
+  </si>
+  <si>
     <t>AVAL</t>
   </si>
   <si>
@@ -446,6 +458,9 @@
     <t>BASE</t>
   </si>
   <si>
+    <t>Baseline Value</t>
+  </si>
+  <si>
     <t>CRIT1FL</t>
   </si>
   <si>
@@ -560,6 +575,9 @@
     <t>PROGRAMMINGCODE</t>
   </si>
   <si>
+    <t>date9.</t>
+  </si>
+  <si>
     <t>Adverse Events Analysis Datasets</t>
   </si>
   <si>
@@ -800,6 +818,9 @@
     <t>ADUR</t>
   </si>
   <si>
+    <t>URSEQ</t>
+  </si>
+  <si>
     <t>UR</t>
   </si>
   <si>
@@ -1080,6 +1101,9 @@
   </si>
   <si>
     <t>ADTTE.PARAM</t>
+  </si>
+  <si>
+    <t>ADUR.PARAM</t>
   </si>
   <si>
     <t>Hardcoded to DISCONTD</t>
@@ -2081,45 +2105,45 @@
         <v>72</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H1" s="38" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="I1" s="38" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
-        <v>295</v>
+        <v>302</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>296</v>
+        <v>303</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>295</v>
+        <v>302</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>297</v>
+        <v>304</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>298</v>
+        <v>305</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>209</v>
+        <v>215</v>
       </c>
       <c r="G2" s="63" t="s">
-        <v>300</v>
+        <v>307</v>
       </c>
       <c r="H2" s="39" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="I2" s="52" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
     </row>
   </sheetData>
@@ -2149,25 +2173,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="34" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="B1" s="35" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="C1" s="53" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="D1" s="55" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="E1" s="34" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.2">
@@ -2239,8 +2263,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B3" sqref="A3:XFD3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="23.1" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2290,15 +2314,15 @@
         <v>9</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>10</v>
@@ -2307,31 +2331,31 @@
         <v>11</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>215</v>
+        <v>221</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="K2"/>
     </row>
     <row r="3" spans="1:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>11</v>
@@ -2340,31 +2364,31 @@
         <v>11</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>0</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>212</v>
+        <v>218</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K3" s="2"/>
     </row>
     <row r="4" spans="1:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>235</v>
+        <v>241</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>342</v>
+        <v>350</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>10</v>
@@ -2373,31 +2397,31 @@
         <v>11</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>347</v>
+        <v>355</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>14</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>343</v>
+        <v>351</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>213</v>
+        <v>219</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>342</v>
+        <v>350</v>
       </c>
       <c r="K4" s="2"/>
     </row>
     <row r="5" spans="1:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>325</v>
+        <v>332</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>325</v>
+        <v>332</v>
       </c>
       <c r="C5" s="28" t="s">
         <v>11</v>
@@ -2406,30 +2430,30 @@
         <v>11</v>
       </c>
       <c r="E5" s="28" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="F5" s="96" t="s">
-        <v>348</v>
+        <v>356</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>0</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>213</v>
+        <v>219</v>
       </c>
       <c r="J5" t="s">
-        <v>325</v>
+        <v>332</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="28" t="s">
-        <v>217</v>
+        <v>223</v>
       </c>
       <c r="B6" s="28" t="s">
-        <v>217</v>
+        <v>223</v>
       </c>
       <c r="C6" s="28" t="s">
         <v>11</v>
@@ -2438,22 +2462,22 @@
         <v>11</v>
       </c>
       <c r="E6" s="28" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="F6" s="43" t="s">
-        <v>299</v>
+        <v>306</v>
       </c>
       <c r="G6" s="28" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="H6" s="28" t="s">
         <v>0</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>213</v>
+        <v>219</v>
       </c>
       <c r="J6" s="30" t="s">
-        <v>217</v>
+        <v>223</v>
       </c>
       <c r="K6" s="30"/>
     </row>
@@ -2467,11 +2491,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q63"/>
+  <dimension ref="A1:Q82"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A18" sqref="A18:XFD36"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="23.1" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2512,7 +2536,7 @@
         <v>3</v>
       </c>
       <c r="G1" s="71" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="H1" s="69" t="s">
         <v>20</v>
@@ -2521,7 +2545,7 @@
         <v>21</v>
       </c>
       <c r="J1" s="72" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="K1" s="69" t="s">
         <v>23</v>
@@ -2542,12 +2566,12 @@
         <v>28</v>
       </c>
       <c r="Q1" s="73" t="s">
-        <v>279</v>
+        <v>286</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="74" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B2" s="75">
         <v>1</v>
@@ -2580,7 +2604,7 @@
     </row>
     <row r="3" spans="1:17" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="74" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B3" s="75">
         <v>2</v>
@@ -2613,7 +2637,7 @@
     </row>
     <row r="4" spans="1:17" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="74" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B4" s="75">
         <v>3</v>
@@ -2643,7 +2667,7 @@
     </row>
     <row r="5" spans="1:17" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="74" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B5" s="75">
         <v>4</v>
@@ -2673,7 +2697,7 @@
     </row>
     <row r="6" spans="1:17" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="74" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B6" s="75">
         <v>5</v>
@@ -2706,7 +2730,7 @@
     </row>
     <row r="7" spans="1:17" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="74" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B7" s="75">
         <v>6</v>
@@ -2739,7 +2763,7 @@
     </row>
     <row r="8" spans="1:17" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="74" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B8" s="75">
         <v>7</v>
@@ -2772,7 +2796,7 @@
     </row>
     <row r="9" spans="1:17" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="74" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B9" s="75">
         <v>8</v>
@@ -2805,32 +2829,32 @@
     </row>
     <row r="10" spans="1:17" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="74" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B10" s="75">
         <v>9</v>
       </c>
       <c r="C10" s="74" t="s">
-        <v>331</v>
+        <v>339</v>
       </c>
       <c r="D10" s="74" t="s">
-        <v>305</v>
+        <v>312</v>
       </c>
       <c r="E10" s="75">
         <v>1</v>
       </c>
       <c r="F10" s="74" t="s">
-        <v>332</v>
+        <v>340</v>
       </c>
       <c r="I10" s="74" t="s">
         <v>32</v>
       </c>
       <c r="J10" s="77"/>
       <c r="L10" s="74" t="s">
-        <v>331</v>
+        <v>339</v>
       </c>
       <c r="M10" s="74" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="N10" s="74" t="s">
         <v>10</v>
@@ -2838,7 +2862,7 @@
     </row>
     <row r="11" spans="1:17" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="74" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B11" s="75">
         <v>10</v>
@@ -2868,13 +2892,13 @@
     </row>
     <row r="12" spans="1:17" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="74" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B12" s="75">
         <v>11</v>
       </c>
       <c r="C12" s="74" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D12" s="74" t="s">
         <v>30</v>
@@ -2883,10 +2907,10 @@
         <v>40</v>
       </c>
       <c r="F12" s="74" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="I12" s="74" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="J12" s="77"/>
       <c r="N12" s="74" t="s">
@@ -2898,13 +2922,13 @@
     </row>
     <row r="13" spans="1:17" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="74" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B13" s="75">
         <v>12</v>
       </c>
       <c r="C13" s="74" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D13" s="74" t="s">
         <v>36</v>
@@ -2913,16 +2937,16 @@
         <v>3</v>
       </c>
       <c r="F13" s="74" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="I13" s="74" t="s">
         <v>32</v>
       </c>
       <c r="L13" s="95" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="M13" s="74" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="N13" s="74" t="s">
         <v>11</v>
@@ -2933,13 +2957,13 @@
     </row>
     <row r="14" spans="1:17" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="74" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B14" s="75">
         <v>13</v>
       </c>
       <c r="C14" s="74" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D14" s="74" t="s">
         <v>36</v>
@@ -2948,14 +2972,14 @@
         <v>8</v>
       </c>
       <c r="F14" s="74" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="I14" s="74" t="s">
         <v>32</v>
       </c>
       <c r="J14" s="77"/>
       <c r="L14" s="74" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="N14" s="74" t="s">
         <v>10</v>
@@ -2966,13 +2990,13 @@
     </row>
     <row r="15" spans="1:17" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="74" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B15" s="75">
         <v>14</v>
       </c>
       <c r="C15" s="74" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D15" s="74" t="s">
         <v>36</v>
@@ -2981,14 +3005,14 @@
         <v>8</v>
       </c>
       <c r="F15" s="74" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="I15" s="74" t="s">
         <v>32</v>
       </c>
       <c r="J15" s="77"/>
       <c r="L15" s="74" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="N15" s="74" t="s">
         <v>10</v>
@@ -2999,43 +3023,43 @@
     </row>
     <row r="16" spans="1:17" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="74" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B16" s="75">
         <v>15</v>
       </c>
       <c r="C16" s="74" t="s">
-        <v>311</v>
+        <v>318</v>
       </c>
       <c r="D16" s="74" t="s">
-        <v>313</v>
+        <v>320</v>
       </c>
       <c r="E16" s="75">
         <v>21</v>
       </c>
       <c r="F16" s="74" t="s">
-        <v>314</v>
+        <v>321</v>
       </c>
       <c r="I16" s="74" t="s">
         <v>32</v>
       </c>
       <c r="J16" s="77"/>
       <c r="L16" s="74" t="s">
-        <v>311</v>
+        <v>318</v>
       </c>
       <c r="M16" s="74" t="s">
-        <v>306</v>
+        <v>313</v>
       </c>
     </row>
     <row r="17" spans="1:17" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="74" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B17" s="75">
         <v>16</v>
       </c>
       <c r="C17" s="74" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D17" s="74" t="s">
         <v>36</v>
@@ -3044,14 +3068,14 @@
         <v>8</v>
       </c>
       <c r="F17" s="74" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="I17" s="74" t="s">
         <v>32</v>
       </c>
       <c r="J17" s="77"/>
       <c r="L17" s="74" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="N17" s="74" t="s">
         <v>10</v>
@@ -3062,12 +3086,12 @@
     </row>
     <row r="18" spans="1:17" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="74" t="s">
-        <v>122</v>
+        <v>241</v>
       </c>
       <c r="B18" s="75">
         <v>1</v>
       </c>
-      <c r="C18" s="74" t="s">
+      <c r="C18" s="78" t="s">
         <v>29</v>
       </c>
       <c r="D18" s="74" t="s">
@@ -3083,7 +3107,7 @@
         <v>1</v>
       </c>
       <c r="I18" s="74" t="s">
-        <v>179</v>
+        <v>243</v>
       </c>
       <c r="J18" s="77"/>
       <c r="N18" s="74" t="s">
@@ -3092,12 +3116,12 @@
     </row>
     <row r="19" spans="1:17" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="74" t="s">
-        <v>122</v>
+        <v>241</v>
       </c>
       <c r="B19" s="75">
         <v>2</v>
       </c>
-      <c r="C19" s="74" t="s">
+      <c r="C19" s="78" t="s">
         <v>33</v>
       </c>
       <c r="D19" s="74" t="s">
@@ -3113,7 +3137,7 @@
         <v>2</v>
       </c>
       <c r="I19" s="74" t="s">
-        <v>179</v>
+        <v>243</v>
       </c>
       <c r="J19" s="77"/>
       <c r="N19" s="74" t="s">
@@ -3122,40 +3146,40 @@
     </row>
     <row r="20" spans="1:17" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="74" t="s">
-        <v>122</v>
+        <v>241</v>
       </c>
       <c r="B20" s="75">
         <v>3</v>
       </c>
-      <c r="C20" s="74" t="s">
-        <v>35</v>
+      <c r="C20" s="78" t="s">
+        <v>242</v>
       </c>
       <c r="D20" s="74" t="s">
         <v>36</v>
       </c>
-      <c r="E20" s="81">
+      <c r="E20" s="75">
         <v>8</v>
       </c>
       <c r="F20" s="74" t="s">
         <v>37</v>
       </c>
       <c r="I20" s="74" t="s">
-        <v>179</v>
+        <v>243</v>
       </c>
       <c r="J20" s="77"/>
       <c r="N20" s="74" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:17" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:17" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="74" t="s">
-        <v>122</v>
+        <v>241</v>
       </c>
       <c r="B21" s="75">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C21" s="78" t="s">
-        <v>125</v>
+        <v>102</v>
       </c>
       <c r="D21" s="74" t="s">
         <v>30</v>
@@ -3164,25 +3188,25 @@
         <v>14</v>
       </c>
       <c r="F21" s="74" t="s">
-        <v>126</v>
+        <v>103</v>
       </c>
       <c r="I21" s="74" t="s">
-        <v>195</v>
-      </c>
-      <c r="J21" s="77"/>
+        <v>201</v>
+      </c>
+      <c r="J21" s="80"/>
       <c r="N21" s="74" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:17" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:17" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="74" t="s">
-        <v>122</v>
+        <v>241</v>
       </c>
       <c r="B22" s="75">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C22" s="78" t="s">
-        <v>123</v>
+        <v>100</v>
       </c>
       <c r="D22" s="74" t="s">
         <v>36</v>
@@ -3191,432 +3215,459 @@
         <v>8</v>
       </c>
       <c r="F22" s="74" t="s">
-        <v>124</v>
+        <v>101</v>
       </c>
       <c r="I22" s="74" t="s">
-        <v>196</v>
-      </c>
-      <c r="J22" s="77"/>
+        <v>202</v>
+      </c>
+      <c r="J22" s="80"/>
       <c r="N22" s="74" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:17" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:17" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="74" t="s">
-        <v>122</v>
+        <v>241</v>
       </c>
       <c r="B23" s="75">
-        <v>6</v>
-      </c>
-      <c r="C23" s="74" t="s">
-        <v>38</v>
+        <v>8</v>
+      </c>
+      <c r="C23" s="78" t="s">
+        <v>104</v>
       </c>
       <c r="D23" s="74" t="s">
         <v>30</v>
       </c>
-      <c r="E23" s="81">
-        <v>50</v>
+      <c r="E23" s="75">
+        <v>8</v>
       </c>
       <c r="F23" s="74" t="s">
-        <v>39</v>
+        <v>105</v>
+      </c>
+      <c r="G23" s="76">
+        <v>3</v>
       </c>
       <c r="I23" s="74" t="s">
-        <v>179</v>
-      </c>
-      <c r="J23" s="77"/>
+        <v>188</v>
+      </c>
+      <c r="J23" s="80"/>
+      <c r="L23" s="95" t="s">
+        <v>334</v>
+      </c>
       <c r="N23" s="74" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="74" t="s">
+        <v>241</v>
+      </c>
+      <c r="B24" s="75">
+        <v>9</v>
+      </c>
+      <c r="C24" s="78" t="s">
+        <v>106</v>
+      </c>
+      <c r="D24" s="74" t="s">
+        <v>30</v>
+      </c>
+      <c r="E24" s="75">
+        <v>61</v>
+      </c>
+      <c r="F24" s="74" t="s">
+        <v>107</v>
+      </c>
+      <c r="I24" s="74" t="s">
+        <v>188</v>
+      </c>
+      <c r="J24" s="80"/>
+      <c r="L24" s="95" t="s">
+        <v>337</v>
+      </c>
+      <c r="N24" s="74" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="74" t="s">
+        <v>241</v>
+      </c>
+      <c r="B25" s="75">
         <v>10</v>
       </c>
-    </row>
-    <row r="24" spans="1:17" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="74" t="s">
-        <v>122</v>
-      </c>
-      <c r="B24" s="75">
-        <v>7</v>
-      </c>
-      <c r="C24" s="74" t="s">
-        <v>40</v>
-      </c>
-      <c r="D24" s="74" t="s">
-        <v>30</v>
-      </c>
-      <c r="E24" s="81">
-        <v>45</v>
-      </c>
-      <c r="F24" s="74" t="s">
-        <v>41</v>
-      </c>
-      <c r="G24" s="76">
-        <v>3</v>
-      </c>
-      <c r="I24" s="74" t="s">
-        <v>179</v>
-      </c>
-      <c r="J24" s="77"/>
-      <c r="M24" s="78" t="s">
-        <v>42</v>
-      </c>
-      <c r="N24" s="74" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="74" t="s">
-        <v>122</v>
-      </c>
-      <c r="B25" s="75">
+      <c r="C25" s="78" t="s">
+        <v>108</v>
+      </c>
+      <c r="D25" s="74" t="s">
+        <v>30</v>
+      </c>
+      <c r="E25" s="75">
+        <v>16</v>
+      </c>
+      <c r="F25" s="74" t="s">
+        <v>109</v>
+      </c>
+      <c r="I25" s="74" t="s">
+        <v>244</v>
+      </c>
+      <c r="J25" s="80"/>
+      <c r="N25" s="74" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="74" t="s">
+        <v>241</v>
+      </c>
+      <c r="B26" s="75">
+        <v>11</v>
+      </c>
+      <c r="C26" s="78" t="s">
+        <v>110</v>
+      </c>
+      <c r="D26" s="74" t="s">
+        <v>36</v>
+      </c>
+      <c r="E26" s="75">
         <v>8</v>
       </c>
-      <c r="C25" s="74" t="s">
-        <v>304</v>
-      </c>
-      <c r="D25" s="74" t="s">
-        <v>30</v>
-      </c>
-      <c r="E25" s="81">
-        <v>3</v>
-      </c>
-      <c r="F25" s="74" t="s">
-        <v>43</v>
-      </c>
-      <c r="G25" s="76"/>
-      <c r="I25" s="74" t="s">
-        <v>179</v>
-      </c>
-      <c r="J25" s="77"/>
-      <c r="M25" s="78"/>
-    </row>
-    <row r="26" spans="1:17" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="74" t="s">
-        <v>122</v>
-      </c>
-      <c r="B26" s="75">
-        <v>9</v>
-      </c>
-      <c r="C26" s="74" t="s">
-        <v>294</v>
-      </c>
-      <c r="D26" s="74" t="s">
-        <v>30</v>
-      </c>
-      <c r="E26" s="81">
-        <v>70</v>
-      </c>
       <c r="F26" s="74" t="s">
-        <v>303</v>
+        <v>111</v>
+      </c>
+      <c r="G26" s="76">
+        <v>4</v>
       </c>
       <c r="I26" s="74" t="s">
-        <v>179</v>
-      </c>
-      <c r="J26" s="77"/>
-      <c r="M26" s="78" t="s">
-        <v>42</v>
-      </c>
+        <v>283</v>
+      </c>
+      <c r="L26" s="80"/>
       <c r="N26" s="74" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="27" spans="1:17" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="74" t="s">
-        <v>122</v>
+        <v>241</v>
       </c>
       <c r="B27" s="75">
-        <v>10</v>
-      </c>
-      <c r="C27" s="74" t="s">
-        <v>316</v>
+        <v>12</v>
+      </c>
+      <c r="C27" s="78" t="s">
+        <v>112</v>
       </c>
       <c r="D27" s="74" t="s">
         <v>30</v>
       </c>
       <c r="E27" s="75">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F27" s="74" t="s">
-        <v>238</v>
-      </c>
-      <c r="G27" s="76">
-        <v>4</v>
+        <v>113</v>
       </c>
       <c r="I27" s="74" t="s">
-        <v>179</v>
+        <v>32</v>
       </c>
       <c r="J27" s="77"/>
+      <c r="L27" s="74" t="s">
+        <v>112</v>
+      </c>
+      <c r="M27" s="74" t="s">
+        <v>84</v>
+      </c>
       <c r="N27" s="74" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="28" spans="1:17" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="74" t="s">
-        <v>122</v>
+        <v>241</v>
       </c>
       <c r="B28" s="75">
+        <v>13</v>
+      </c>
+      <c r="C28" s="78" t="s">
+        <v>114</v>
+      </c>
+      <c r="D28" s="74" t="s">
+        <v>36</v>
+      </c>
+      <c r="E28" s="75">
+        <v>8</v>
+      </c>
+      <c r="F28" s="74" t="s">
+        <v>115</v>
+      </c>
+      <c r="G28" s="76">
+        <v>5</v>
+      </c>
+      <c r="I28" s="74" t="s">
+        <v>32</v>
+      </c>
+      <c r="J28" s="77"/>
+      <c r="K28" s="74" t="s">
+        <v>161</v>
+      </c>
+      <c r="L28" s="74" t="s">
+        <v>114</v>
+      </c>
+      <c r="N28" s="74" t="s">
         <v>11</v>
-      </c>
-      <c r="C28" s="74" t="s">
-        <v>315</v>
-      </c>
-      <c r="D28" s="74" t="s">
-        <v>30</v>
-      </c>
-      <c r="E28" s="75">
-        <v>10</v>
-      </c>
-      <c r="F28" s="74" t="s">
-        <v>239</v>
-      </c>
-      <c r="I28" s="74" t="s">
-        <v>179</v>
-      </c>
-      <c r="J28" s="77"/>
-      <c r="N28" s="74" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="29" spans="1:17" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="74" t="s">
-        <v>122</v>
+        <v>241</v>
       </c>
       <c r="B29" s="75">
-        <v>12</v>
-      </c>
-      <c r="C29" s="74" t="s">
-        <v>44</v>
+        <v>14</v>
+      </c>
+      <c r="C29" s="78" t="s">
+        <v>116</v>
       </c>
       <c r="D29" s="74" t="s">
-        <v>30</v>
-      </c>
-      <c r="E29" s="82">
-        <v>20</v>
+        <v>36</v>
+      </c>
+      <c r="E29" s="75">
+        <v>8</v>
       </c>
       <c r="F29" s="74" t="s">
-        <v>45</v>
+        <v>117</v>
       </c>
       <c r="I29" s="74" t="s">
-        <v>179</v>
+        <v>32</v>
       </c>
       <c r="J29" s="77"/>
+      <c r="L29" s="74" t="s">
+        <v>116</v>
+      </c>
       <c r="N29" s="74" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="30" spans="1:17" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="74" t="s">
-        <v>122</v>
+        <v>241</v>
       </c>
       <c r="B30" s="75">
-        <v>13</v>
-      </c>
-      <c r="C30" s="74" t="s">
-        <v>46</v>
+        <v>15</v>
+      </c>
+      <c r="C30" s="78" t="s">
+        <v>330</v>
       </c>
       <c r="D30" s="74" t="s">
-        <v>30</v>
-      </c>
-      <c r="E30" s="82">
-        <v>3</v>
+        <v>36</v>
+      </c>
+      <c r="E30" s="75">
+        <v>8</v>
       </c>
       <c r="F30" s="74" t="s">
-        <v>47</v>
+        <v>331</v>
       </c>
       <c r="I30" s="74" t="s">
-        <v>179</v>
+        <v>32</v>
       </c>
       <c r="J30" s="77"/>
-      <c r="N30" s="74" t="s">
-        <v>11</v>
+      <c r="L30" s="74" t="s">
+        <v>330</v>
       </c>
     </row>
     <row r="31" spans="1:17" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="74" t="s">
-        <v>122</v>
+        <v>241</v>
       </c>
       <c r="B31" s="75">
-        <v>14</v>
-      </c>
-      <c r="C31" s="74" t="s">
-        <v>48</v>
+        <v>16</v>
+      </c>
+      <c r="C31" s="78" t="s">
+        <v>118</v>
       </c>
       <c r="D31" s="74" t="s">
-        <v>30</v>
-      </c>
-      <c r="E31" s="82">
-        <v>20</v>
+        <v>36</v>
+      </c>
+      <c r="E31" s="75">
+        <v>8</v>
       </c>
       <c r="F31" s="74" t="s">
-        <v>49</v>
+        <v>119</v>
       </c>
       <c r="I31" s="74" t="s">
-        <v>179</v>
-      </c>
-      <c r="J31" s="77"/>
+        <v>243</v>
+      </c>
+      <c r="L31" s="78"/>
       <c r="N31" s="74" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="32" spans="1:17" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="74" t="s">
-        <v>122</v>
+        <v>241</v>
       </c>
       <c r="B32" s="75">
-        <v>15</v>
-      </c>
-      <c r="C32" s="74" t="s">
-        <v>50</v>
+        <v>17</v>
+      </c>
+      <c r="C32" s="78" t="s">
+        <v>120</v>
       </c>
       <c r="D32" s="74" t="s">
         <v>30</v>
       </c>
-      <c r="E32" s="82">
-        <v>20</v>
+      <c r="E32" s="75">
+        <v>12</v>
       </c>
       <c r="F32" s="74" t="s">
-        <v>51</v>
+        <v>142</v>
       </c>
       <c r="I32" s="74" t="s">
-        <v>179</v>
-      </c>
-      <c r="J32" s="77"/>
+        <v>243</v>
+      </c>
+      <c r="L32" s="78"/>
       <c r="N32" s="74" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="33" spans="1:14" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="74" t="s">
-        <v>217</v>
+        <v>241</v>
       </c>
       <c r="B33" s="75">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="C33" s="78" t="s">
-        <v>29</v>
+        <v>121</v>
       </c>
       <c r="D33" s="74" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="E33" s="75">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="F33" s="74" t="s">
-        <v>31</v>
-      </c>
-      <c r="G33" s="76">
-        <v>1</v>
+        <v>122</v>
       </c>
       <c r="I33" s="74" t="s">
-        <v>1</v>
-      </c>
-      <c r="J33" s="77"/>
+        <v>32</v>
+      </c>
+      <c r="L33" s="78" t="s">
+        <v>121</v>
+      </c>
       <c r="N33" s="74" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="34" spans="1:14" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="74" t="s">
-        <v>217</v>
+        <v>241</v>
       </c>
       <c r="B34" s="75">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="C34" s="78" t="s">
-        <v>33</v>
+        <v>343</v>
       </c>
       <c r="D34" s="74" t="s">
         <v>30</v>
       </c>
       <c r="E34" s="75">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="F34" s="74" t="s">
-        <v>34</v>
-      </c>
-      <c r="G34" s="76">
-        <v>2</v>
+        <v>344</v>
       </c>
       <c r="I34" s="74" t="s">
-        <v>1</v>
-      </c>
-      <c r="J34" s="77"/>
-      <c r="N34" s="74" t="s">
-        <v>10</v>
+        <v>32</v>
+      </c>
+      <c r="L34" s="78" t="s">
+        <v>343</v>
+      </c>
+      <c r="M34" s="74" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="35" spans="1:14" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="74" t="s">
-        <v>217</v>
+        <v>241</v>
       </c>
       <c r="B35" s="75">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="C35" s="78" t="s">
-        <v>56</v>
+        <v>294</v>
       </c>
       <c r="D35" s="74" t="s">
         <v>36</v>
       </c>
       <c r="E35" s="75">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="F35" s="74" t="s">
-        <v>56</v>
+        <v>295</v>
       </c>
       <c r="I35" s="74" t="s">
-        <v>1</v>
-      </c>
-      <c r="J35" s="77"/>
+        <v>32</v>
+      </c>
+      <c r="L35" s="78" t="s">
+        <v>294</v>
+      </c>
+      <c r="M35" s="74" t="s">
+        <v>329</v>
+      </c>
       <c r="N35" s="74" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="36" spans="1:14" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="74" t="s">
-        <v>217</v>
+        <v>241</v>
       </c>
       <c r="B36" s="75">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="C36" s="78" t="s">
-        <v>61</v>
+        <v>125</v>
       </c>
       <c r="D36" s="74" t="s">
         <v>30</v>
       </c>
       <c r="E36" s="75">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="F36" s="74" t="s">
-        <v>62</v>
+        <v>126</v>
       </c>
       <c r="I36" s="74" t="s">
-        <v>1</v>
-      </c>
-      <c r="J36" s="77"/>
+        <v>32</v>
+      </c>
+      <c r="L36" s="78" t="s">
+        <v>125</v>
+      </c>
       <c r="N36" s="74" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="37" spans="1:14" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="74" t="s">
-        <v>217</v>
+        <v>127</v>
       </c>
       <c r="B37" s="75">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C37" s="74" t="s">
-        <v>63</v>
+        <v>29</v>
       </c>
       <c r="D37" s="74" t="s">
         <v>30</v>
       </c>
       <c r="E37" s="75">
-        <v>45</v>
+        <v>15</v>
       </c>
       <c r="F37" s="74" t="s">
-        <v>64</v>
+        <v>31</v>
+      </c>
+      <c r="G37" s="76">
+        <v>1</v>
       </c>
       <c r="I37" s="74" t="s">
-        <v>1</v>
+        <v>185</v>
       </c>
       <c r="J37" s="77"/>
       <c r="N37" s="74" t="s">
@@ -3625,109 +3676,97 @@
     </row>
     <row r="38" spans="1:14" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="74" t="s">
-        <v>217</v>
+        <v>127</v>
       </c>
       <c r="B38" s="75">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C38" s="74" t="s">
-        <v>218</v>
+        <v>33</v>
       </c>
       <c r="D38" s="74" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="E38" s="75">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="F38" s="74" t="s">
-        <v>220</v>
+        <v>34</v>
+      </c>
+      <c r="G38" s="76">
+        <v>2</v>
       </c>
       <c r="I38" s="74" t="s">
-        <v>32</v>
+        <v>185</v>
       </c>
       <c r="J38" s="77"/>
-      <c r="L38" s="74" t="s">
-        <v>218</v>
-      </c>
       <c r="N38" s="74" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="39" spans="1:14" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="74" t="s">
-        <v>217</v>
+        <v>127</v>
       </c>
       <c r="B39" s="75">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C39" s="74" t="s">
-        <v>219</v>
+        <v>35</v>
       </c>
       <c r="D39" s="74" t="s">
-        <v>30</v>
-      </c>
-      <c r="E39" s="75">
-        <v>30</v>
+        <v>36</v>
+      </c>
+      <c r="E39" s="81">
+        <v>8</v>
       </c>
       <c r="F39" s="74" t="s">
-        <v>221</v>
+        <v>37</v>
       </c>
       <c r="I39" s="74" t="s">
-        <v>32</v>
+        <v>185</v>
       </c>
       <c r="J39" s="77"/>
-      <c r="L39" s="74" t="s">
-        <v>219</v>
-      </c>
-      <c r="M39" s="74" t="s">
-        <v>219</v>
-      </c>
       <c r="N39" s="74" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="40" spans="1:14" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="74" t="s">
-        <v>217</v>
+        <v>127</v>
       </c>
       <c r="B40" s="75">
-        <v>10</v>
-      </c>
-      <c r="C40" s="74" t="s">
-        <v>223</v>
+        <v>4</v>
+      </c>
+      <c r="C40" s="78" t="s">
+        <v>130</v>
       </c>
       <c r="D40" s="74" t="s">
         <v>30</v>
       </c>
-      <c r="E40" s="75">
-        <v>30</v>
+      <c r="E40" s="81">
+        <v>14</v>
       </c>
       <c r="F40" s="74" t="s">
-        <v>224</v>
+        <v>131</v>
       </c>
       <c r="I40" s="74" t="s">
-        <v>32</v>
+        <v>201</v>
       </c>
       <c r="J40" s="77"/>
-      <c r="L40" s="74" t="s">
-        <v>223</v>
-      </c>
-      <c r="M40" s="74" t="s">
-        <v>223</v>
-      </c>
       <c r="N40" s="74" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="41" spans="1:14" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="74" t="s">
-        <v>217</v>
+        <v>127</v>
       </c>
       <c r="B41" s="75">
-        <v>11</v>
-      </c>
-      <c r="C41" s="74" t="s">
-        <v>89</v>
+        <v>5</v>
+      </c>
+      <c r="C41" s="78" t="s">
+        <v>128</v>
       </c>
       <c r="D41" s="74" t="s">
         <v>36</v>
@@ -3736,71 +3775,71 @@
         <v>8</v>
       </c>
       <c r="F41" s="74" t="s">
-        <v>222</v>
+        <v>129</v>
       </c>
       <c r="I41" s="74" t="s">
-        <v>32</v>
+        <v>202</v>
       </c>
       <c r="J41" s="77"/>
-      <c r="L41" s="74" t="s">
-        <v>89</v>
-      </c>
       <c r="N41" s="74" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:14" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="74" t="s">
-        <v>217</v>
+        <v>127</v>
       </c>
       <c r="B42" s="75">
-        <v>12</v>
-      </c>
-      <c r="C42" s="78" t="s">
-        <v>101</v>
+        <v>6</v>
+      </c>
+      <c r="C42" s="74" t="s">
+        <v>38</v>
       </c>
       <c r="D42" s="74" t="s">
         <v>30</v>
       </c>
       <c r="E42" s="81">
-        <v>14</v>
+        <v>50</v>
       </c>
       <c r="F42" s="74" t="s">
-        <v>102</v>
+        <v>39</v>
       </c>
       <c r="I42" s="74" t="s">
-        <v>181</v>
-      </c>
-      <c r="J42" s="80"/>
+        <v>185</v>
+      </c>
+      <c r="J42" s="77"/>
       <c r="N42" s="74" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="43" spans="1:14" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="74" t="s">
-        <v>217</v>
+        <v>127</v>
       </c>
       <c r="B43" s="75">
-        <v>13</v>
-      </c>
-      <c r="C43" s="78" t="s">
-        <v>99</v>
+        <v>7</v>
+      </c>
+      <c r="C43" s="74" t="s">
+        <v>40</v>
       </c>
       <c r="D43" s="74" t="s">
-        <v>36</v>
-      </c>
-      <c r="E43" s="75">
-        <v>8</v>
+        <v>30</v>
+      </c>
+      <c r="E43" s="81">
+        <v>45</v>
       </c>
       <c r="F43" s="74" t="s">
-        <v>100</v>
+        <v>41</v>
+      </c>
+      <c r="G43" s="76">
+        <v>3</v>
       </c>
       <c r="I43" s="74" t="s">
-        <v>32</v>
-      </c>
-      <c r="J43" s="80"/>
-      <c r="L43" s="74" t="s">
-        <v>99</v>
+        <v>185</v>
+      </c>
+      <c r="J43" s="77"/>
+      <c r="M43" s="78" t="s">
+        <v>42</v>
       </c>
       <c r="N43" s="74" t="s">
         <v>10</v>
@@ -3808,449 +3847,457 @@
     </row>
     <row r="44" spans="1:14" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="74" t="s">
-        <v>325</v>
+        <v>127</v>
       </c>
       <c r="B44" s="75">
-        <v>1</v>
-      </c>
-      <c r="C44" s="78" t="s">
-        <v>29</v>
+        <v>8</v>
+      </c>
+      <c r="C44" s="74" t="s">
+        <v>311</v>
       </c>
       <c r="D44" s="74" t="s">
         <v>30</v>
       </c>
-      <c r="E44" s="75">
-        <v>15</v>
+      <c r="E44" s="81">
+        <v>3</v>
       </c>
       <c r="F44" s="74" t="s">
-        <v>31</v>
-      </c>
-      <c r="G44" s="76">
-        <v>1</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="G44" s="76"/>
       <c r="I44" s="74" t="s">
-        <v>236</v>
+        <v>185</v>
       </c>
       <c r="J44" s="77"/>
-      <c r="N44" s="74" t="s">
-        <v>10</v>
-      </c>
+      <c r="M44" s="78"/>
     </row>
     <row r="45" spans="1:14" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="74" t="s">
-        <v>325</v>
+        <v>127</v>
       </c>
       <c r="B45" s="75">
-        <v>2</v>
-      </c>
-      <c r="C45" s="78" t="s">
-        <v>33</v>
+        <v>9</v>
+      </c>
+      <c r="C45" s="74" t="s">
+        <v>301</v>
       </c>
       <c r="D45" s="74" t="s">
         <v>30</v>
       </c>
-      <c r="E45" s="75">
-        <v>25</v>
+      <c r="E45" s="81">
+        <v>70</v>
       </c>
       <c r="F45" s="74" t="s">
-        <v>34</v>
-      </c>
-      <c r="G45" s="76">
-        <v>2</v>
+        <v>310</v>
       </c>
       <c r="I45" s="74" t="s">
-        <v>236</v>
+        <v>185</v>
       </c>
       <c r="J45" s="77"/>
+      <c r="M45" s="78" t="s">
+        <v>42</v>
+      </c>
       <c r="N45" s="74" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="46" spans="1:14" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="74" t="s">
-        <v>325</v>
+        <v>127</v>
       </c>
       <c r="B46" s="75">
-        <v>3</v>
-      </c>
-      <c r="C46" s="78" t="s">
-        <v>101</v>
+        <v>10</v>
+      </c>
+      <c r="C46" s="74" t="s">
+        <v>323</v>
       </c>
       <c r="D46" s="74" t="s">
         <v>30</v>
       </c>
-      <c r="E46" s="81">
-        <v>14</v>
+      <c r="E46" s="75">
+        <v>10</v>
       </c>
       <c r="F46" s="74" t="s">
-        <v>102</v>
+        <v>245</v>
+      </c>
+      <c r="G46" s="76">
+        <v>4</v>
       </c>
       <c r="I46" s="74" t="s">
-        <v>195</v>
-      </c>
-      <c r="J46" s="80"/>
+        <v>185</v>
+      </c>
+      <c r="J46" s="77"/>
       <c r="N46" s="74" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="74" t="s">
+        <v>127</v>
+      </c>
+      <c r="B47" s="75">
         <v>11</v>
       </c>
-    </row>
-    <row r="47" spans="1:14" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="74" t="s">
-        <v>325</v>
-      </c>
-      <c r="B47" s="75">
-        <v>4</v>
-      </c>
-      <c r="C47" s="78" t="s">
-        <v>99</v>
+      <c r="C47" s="74" t="s">
+        <v>322</v>
       </c>
       <c r="D47" s="74" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="E47" s="75">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F47" s="74" t="s">
-        <v>100</v>
+        <v>246</v>
       </c>
       <c r="I47" s="74" t="s">
-        <v>196</v>
-      </c>
-      <c r="J47" s="80"/>
+        <v>185</v>
+      </c>
+      <c r="J47" s="77"/>
       <c r="N47" s="74" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="48" spans="1:14" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="74" t="s">
-        <v>325</v>
+        <v>127</v>
       </c>
       <c r="B48" s="75">
-        <v>5</v>
-      </c>
-      <c r="C48" s="78" t="s">
-        <v>103</v>
+        <v>12</v>
+      </c>
+      <c r="C48" s="74" t="s">
+        <v>44</v>
       </c>
       <c r="D48" s="74" t="s">
         <v>30</v>
       </c>
-      <c r="E48" s="75">
-        <v>8</v>
+      <c r="E48" s="82">
+        <v>20</v>
       </c>
       <c r="F48" s="74" t="s">
-        <v>104</v>
-      </c>
-      <c r="G48" s="76"/>
+        <v>45</v>
+      </c>
       <c r="I48" s="74" t="s">
-        <v>182</v>
-      </c>
-      <c r="J48" s="80"/>
-      <c r="L48" s="95" t="s">
-        <v>328</v>
-      </c>
+        <v>185</v>
+      </c>
+      <c r="J48" s="77"/>
       <c r="N48" s="74" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="49" spans="1:14" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="74" t="s">
-        <v>325</v>
+        <v>127</v>
       </c>
       <c r="B49" s="75">
-        <v>6</v>
-      </c>
-      <c r="C49" s="78" t="s">
-        <v>105</v>
+        <v>13</v>
+      </c>
+      <c r="C49" s="74" t="s">
+        <v>46</v>
       </c>
       <c r="D49" s="74" t="s">
         <v>30</v>
       </c>
-      <c r="E49" s="75">
-        <v>61</v>
+      <c r="E49" s="82">
+        <v>3</v>
       </c>
       <c r="F49" s="74" t="s">
-        <v>106</v>
+        <v>47</v>
       </c>
       <c r="I49" s="74" t="s">
-        <v>182</v>
-      </c>
-      <c r="J49" s="80"/>
-      <c r="L49" s="95" t="s">
-        <v>329</v>
-      </c>
+        <v>185</v>
+      </c>
+      <c r="J49" s="77"/>
       <c r="N49" s="74" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="50" spans="1:14" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="74" t="s">
-        <v>325</v>
+        <v>127</v>
       </c>
       <c r="B50" s="75">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C50" s="74" t="s">
-        <v>114</v>
+        <v>48</v>
       </c>
       <c r="D50" s="74" t="s">
-        <v>36</v>
-      </c>
-      <c r="E50" s="75">
-        <v>8</v>
+        <v>30</v>
+      </c>
+      <c r="E50" s="82">
+        <v>20</v>
       </c>
       <c r="F50" s="74" t="s">
-        <v>115</v>
+        <v>49</v>
       </c>
       <c r="I50" s="74" t="s">
-        <v>32</v>
-      </c>
-      <c r="L50" s="74" t="s">
-        <v>323</v>
+        <v>185</v>
+      </c>
+      <c r="J50" s="77"/>
+      <c r="N50" s="74" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="51" spans="1:14" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="74" t="s">
-        <v>325</v>
+        <v>127</v>
       </c>
       <c r="B51" s="75">
-        <v>8</v>
-      </c>
-      <c r="C51" s="78" t="s">
-        <v>318</v>
+        <v>15</v>
+      </c>
+      <c r="C51" s="74" t="s">
+        <v>50</v>
       </c>
       <c r="D51" s="74" t="s">
-        <v>312</v>
-      </c>
-      <c r="E51" s="75">
-        <v>3</v>
+        <v>30</v>
+      </c>
+      <c r="E51" s="82">
+        <v>20</v>
       </c>
       <c r="F51" s="74" t="s">
-        <v>320</v>
+        <v>51</v>
       </c>
       <c r="I51" s="74" t="s">
-        <v>32</v>
-      </c>
-      <c r="L51" s="78" t="s">
-        <v>318</v>
+        <v>185</v>
+      </c>
+      <c r="J51" s="77"/>
+      <c r="N51" s="74" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="52" spans="1:14" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="74" t="s">
-        <v>325</v>
+        <v>223</v>
       </c>
       <c r="B52" s="75">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C52" s="78" t="s">
-        <v>319</v>
+        <v>29</v>
       </c>
       <c r="D52" s="74" t="s">
-        <v>313</v>
+        <v>30</v>
       </c>
       <c r="E52" s="75">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F52" s="74" t="s">
-        <v>321</v>
+        <v>31</v>
+      </c>
+      <c r="G52" s="76">
+        <v>1</v>
       </c>
       <c r="I52" s="74" t="s">
-        <v>32</v>
-      </c>
-      <c r="L52" s="78" t="s">
-        <v>319</v>
+        <v>1</v>
+      </c>
+      <c r="J52" s="77"/>
+      <c r="N52" s="74" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="53" spans="1:14" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="74" t="s">
-        <v>342</v>
+        <v>223</v>
       </c>
       <c r="B53" s="75">
+        <v>2</v>
+      </c>
+      <c r="C53" s="78" t="s">
+        <v>33</v>
+      </c>
+      <c r="D53" s="74" t="s">
+        <v>30</v>
+      </c>
+      <c r="E53" s="75">
+        <v>25</v>
+      </c>
+      <c r="F53" s="74" t="s">
+        <v>34</v>
+      </c>
+      <c r="G53" s="76">
+        <v>2</v>
+      </c>
+      <c r="I53" s="74" t="s">
         <v>1</v>
       </c>
-      <c r="C53" s="74" t="s">
-        <v>29</v>
-      </c>
-      <c r="D53" s="74" t="s">
-        <v>30</v>
-      </c>
-      <c r="E53" s="75">
-        <v>15</v>
-      </c>
-      <c r="F53" s="74" t="s">
-        <v>31</v>
-      </c>
-      <c r="G53" s="79">
-        <v>1</v>
-      </c>
-      <c r="I53" s="74" t="s">
-        <v>236</v>
-      </c>
+      <c r="J53" s="77"/>
       <c r="N53" s="74" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="54" spans="1:14" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="74" t="s">
-        <v>342</v>
+        <v>223</v>
       </c>
       <c r="B54" s="75">
-        <v>2</v>
-      </c>
-      <c r="C54" s="74" t="s">
-        <v>33</v>
+        <v>5</v>
+      </c>
+      <c r="C54" s="78" t="s">
+        <v>56</v>
       </c>
       <c r="D54" s="74" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="E54" s="75">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="F54" s="74" t="s">
-        <v>34</v>
-      </c>
-      <c r="G54" s="79">
-        <v>2</v>
+        <v>56</v>
       </c>
       <c r="I54" s="74" t="s">
-        <v>236</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="J54" s="77"/>
       <c r="N54" s="74" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="55" spans="1:14" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="74" t="s">
-        <v>342</v>
+        <v>223</v>
       </c>
       <c r="B55" s="75">
+        <v>6</v>
+      </c>
+      <c r="C55" s="78" t="s">
+        <v>61</v>
+      </c>
+      <c r="D55" s="74" t="s">
+        <v>30</v>
+      </c>
+      <c r="E55" s="75">
         <v>3</v>
       </c>
-      <c r="C55" s="74" t="s">
-        <v>101</v>
-      </c>
-      <c r="D55" s="74" t="s">
-        <v>30</v>
-      </c>
-      <c r="E55" s="75">
-        <v>14</v>
-      </c>
       <c r="F55" s="74" t="s">
-        <v>102</v>
+        <v>62</v>
       </c>
       <c r="I55" s="74" t="s">
-        <v>195</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="J55" s="77"/>
       <c r="N55" s="74" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="56" spans="1:14" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="74" t="s">
-        <v>342</v>
+        <v>223</v>
       </c>
       <c r="B56" s="75">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C56" s="74" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="D56" s="74" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="E56" s="75">
-        <v>8</v>
+        <v>45</v>
       </c>
       <c r="F56" s="74" t="s">
-        <v>100</v>
+        <v>64</v>
       </c>
       <c r="I56" s="74" t="s">
-        <v>196</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="J56" s="77"/>
       <c r="N56" s="74" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="57" spans="1:14" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="74" t="s">
-        <v>342</v>
+        <v>223</v>
       </c>
       <c r="B57" s="75">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C57" s="74" t="s">
-        <v>103</v>
+        <v>224</v>
       </c>
       <c r="D57" s="74" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="E57" s="75">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="F57" s="74" t="s">
-        <v>104</v>
+        <v>226</v>
       </c>
       <c r="I57" s="74" t="s">
-        <v>182</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="J57" s="77"/>
       <c r="L57" s="74" t="s">
-        <v>328</v>
+        <v>224</v>
       </c>
       <c r="N57" s="74" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="58" spans="1:14" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="74" t="s">
-        <v>342</v>
+        <v>223</v>
       </c>
       <c r="B58" s="75">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C58" s="74" t="s">
-        <v>105</v>
+        <v>225</v>
       </c>
       <c r="D58" s="74" t="s">
         <v>30</v>
       </c>
       <c r="E58" s="75">
-        <v>61</v>
+        <v>30</v>
       </c>
       <c r="F58" s="74" t="s">
-        <v>106</v>
+        <v>227</v>
       </c>
       <c r="I58" s="74" t="s">
-        <v>182</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="J58" s="77"/>
       <c r="L58" s="74" t="s">
-        <v>329</v>
+        <v>225</v>
+      </c>
+      <c r="M58" s="74" t="s">
+        <v>225</v>
       </c>
       <c r="N58" s="74" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="59" spans="1:14" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="74" t="s">
-        <v>342</v>
+        <v>223</v>
       </c>
       <c r="B59" s="75">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C59" s="74" t="s">
-        <v>114</v>
+        <v>229</v>
       </c>
       <c r="D59" s="74" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="E59" s="75">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="F59" s="74" t="s">
-        <v>115</v>
+        <v>230</v>
       </c>
       <c r="I59" s="74" t="s">
         <v>32</v>
       </c>
+      <c r="J59" s="77"/>
       <c r="L59" s="74" t="s">
-        <v>344</v>
+        <v>229</v>
+      </c>
+      <c r="M59" s="74" t="s">
+        <v>229</v>
       </c>
       <c r="N59" s="74" t="s">
         <v>10</v>
@@ -4258,66 +4305,70 @@
     </row>
     <row r="60" spans="1:14" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="74" t="s">
-        <v>342</v>
+        <v>223</v>
       </c>
       <c r="B60" s="75">
+        <v>11</v>
+      </c>
+      <c r="C60" s="74" t="s">
+        <v>90</v>
+      </c>
+      <c r="D60" s="74" t="s">
+        <v>36</v>
+      </c>
+      <c r="E60" s="75">
         <v>8</v>
       </c>
-      <c r="C60" s="78" t="s">
-        <v>116</v>
-      </c>
-      <c r="D60" s="74" t="s">
-        <v>30</v>
-      </c>
-      <c r="E60" s="75">
+      <c r="F60" s="74" t="s">
+        <v>228</v>
+      </c>
+      <c r="I60" s="74" t="s">
+        <v>32</v>
+      </c>
+      <c r="J60" s="77"/>
+      <c r="L60" s="74" t="s">
+        <v>90</v>
+      </c>
+      <c r="N60" s="74" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="74" t="s">
+        <v>223</v>
+      </c>
+      <c r="B61" s="75">
         <v>12</v>
       </c>
-      <c r="F60" s="74" t="s">
-        <v>137</v>
-      </c>
-      <c r="I60" s="74" t="s">
-        <v>346</v>
-      </c>
-      <c r="L60" s="78"/>
-      <c r="N60" s="74" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="61" spans="1:14" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="74" t="s">
-        <v>342</v>
-      </c>
-      <c r="B61" s="75">
-        <v>9</v>
-      </c>
-      <c r="C61" s="74" t="s">
-        <v>107</v>
+      <c r="C61" s="78" t="s">
+        <v>102</v>
       </c>
       <c r="D61" s="74" t="s">
         <v>30</v>
       </c>
-      <c r="E61" s="75">
-        <v>16</v>
+      <c r="E61" s="81">
+        <v>14</v>
       </c>
       <c r="F61" s="74" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="I61" s="74" t="s">
-        <v>237</v>
-      </c>
+        <v>187</v>
+      </c>
+      <c r="J61" s="80"/>
       <c r="N61" s="74" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="62" spans="1:14" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:14" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="74" t="s">
-        <v>342</v>
+        <v>223</v>
       </c>
       <c r="B62" s="75">
-        <v>10</v>
-      </c>
-      <c r="C62" s="74" t="s">
-        <v>109</v>
+        <v>13</v>
+      </c>
+      <c r="C62" s="78" t="s">
+        <v>100</v>
       </c>
       <c r="D62" s="74" t="s">
         <v>36</v>
@@ -4326,45 +4377,578 @@
         <v>8</v>
       </c>
       <c r="F62" s="74" t="s">
-        <v>110</v>
-      </c>
-      <c r="G62" s="79">
-        <v>4</v>
+        <v>101</v>
       </c>
       <c r="I62" s="74" t="s">
-        <v>276</v>
+        <v>32</v>
+      </c>
+      <c r="J62" s="80"/>
+      <c r="L62" s="74" t="s">
+        <v>100</v>
       </c>
       <c r="N62" s="74" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="63" spans="1:14" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="74" t="s">
-        <v>342</v>
+        <v>332</v>
       </c>
       <c r="B63" s="75">
+        <v>1</v>
+      </c>
+      <c r="C63" s="78" t="s">
+        <v>29</v>
+      </c>
+      <c r="D63" s="74" t="s">
+        <v>30</v>
+      </c>
+      <c r="E63" s="75">
+        <v>15</v>
+      </c>
+      <c r="F63" s="74" t="s">
+        <v>31</v>
+      </c>
+      <c r="G63" s="76">
+        <v>1</v>
+      </c>
+      <c r="I63" s="74" t="s">
+        <v>243</v>
+      </c>
+      <c r="J63" s="77"/>
+      <c r="N63" s="74" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="74" t="s">
+        <v>332</v>
+      </c>
+      <c r="B64" s="75">
+        <v>2</v>
+      </c>
+      <c r="C64" s="78" t="s">
+        <v>33</v>
+      </c>
+      <c r="D64" s="74" t="s">
+        <v>30</v>
+      </c>
+      <c r="E64" s="75">
+        <v>25</v>
+      </c>
+      <c r="F64" s="74" t="s">
+        <v>34</v>
+      </c>
+      <c r="G64" s="76">
+        <v>2</v>
+      </c>
+      <c r="I64" s="74" t="s">
+        <v>243</v>
+      </c>
+      <c r="J64" s="77"/>
+      <c r="N64" s="74" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="74" t="s">
+        <v>332</v>
+      </c>
+      <c r="B65" s="75">
+        <v>3</v>
+      </c>
+      <c r="C65" s="78" t="s">
+        <v>102</v>
+      </c>
+      <c r="D65" s="74" t="s">
+        <v>30</v>
+      </c>
+      <c r="E65" s="81">
+        <v>14</v>
+      </c>
+      <c r="F65" s="74" t="s">
+        <v>103</v>
+      </c>
+      <c r="I65" s="74" t="s">
+        <v>201</v>
+      </c>
+      <c r="J65" s="80"/>
+      <c r="N65" s="74" t="s">
         <v>11</v>
       </c>
-      <c r="C63" s="78" t="s">
+    </row>
+    <row r="66" spans="1:14" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="74" t="s">
+        <v>332</v>
+      </c>
+      <c r="B66" s="75">
+        <v>4</v>
+      </c>
+      <c r="C66" s="78" t="s">
+        <v>100</v>
+      </c>
+      <c r="D66" s="74" t="s">
+        <v>36</v>
+      </c>
+      <c r="E66" s="75">
+        <v>8</v>
+      </c>
+      <c r="F66" s="74" t="s">
+        <v>101</v>
+      </c>
+      <c r="I66" s="74" t="s">
+        <v>202</v>
+      </c>
+      <c r="J66" s="80"/>
+      <c r="N66" s="74" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="74" t="s">
+        <v>332</v>
+      </c>
+      <c r="B67" s="75">
+        <v>5</v>
+      </c>
+      <c r="C67" s="78" t="s">
+        <v>104</v>
+      </c>
+      <c r="D67" s="74" t="s">
+        <v>30</v>
+      </c>
+      <c r="E67" s="75">
+        <v>8</v>
+      </c>
+      <c r="F67" s="74" t="s">
+        <v>105</v>
+      </c>
+      <c r="G67" s="76"/>
+      <c r="I67" s="74" t="s">
+        <v>188</v>
+      </c>
+      <c r="J67" s="80"/>
+      <c r="L67" s="95" t="s">
         <v>335</v>
       </c>
-      <c r="D63" s="74" t="s">
-        <v>30</v>
-      </c>
-      <c r="E63" s="75">
+      <c r="N67" s="74" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="74" t="s">
+        <v>332</v>
+      </c>
+      <c r="B68" s="75">
+        <v>6</v>
+      </c>
+      <c r="C68" s="78" t="s">
+        <v>106</v>
+      </c>
+      <c r="D68" s="74" t="s">
+        <v>30</v>
+      </c>
+      <c r="E68" s="75">
+        <v>61</v>
+      </c>
+      <c r="F68" s="74" t="s">
+        <v>107</v>
+      </c>
+      <c r="I68" s="74" t="s">
+        <v>188</v>
+      </c>
+      <c r="J68" s="80"/>
+      <c r="L68" s="95" t="s">
+        <v>336</v>
+      </c>
+      <c r="N68" s="74" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="74" t="s">
+        <v>332</v>
+      </c>
+      <c r="B69" s="75">
+        <v>7</v>
+      </c>
+      <c r="C69" s="74" t="s">
+        <v>118</v>
+      </c>
+      <c r="D69" s="74" t="s">
+        <v>36</v>
+      </c>
+      <c r="E69" s="75">
+        <v>8</v>
+      </c>
+      <c r="F69" s="74" t="s">
+        <v>119</v>
+      </c>
+      <c r="I69" s="74" t="s">
+        <v>32</v>
+      </c>
+      <c r="L69" s="74" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="74" t="s">
+        <v>332</v>
+      </c>
+      <c r="B70" s="75">
+        <v>8</v>
+      </c>
+      <c r="C70" s="78" t="s">
+        <v>325</v>
+      </c>
+      <c r="D70" s="74" t="s">
+        <v>319</v>
+      </c>
+      <c r="E70" s="75">
+        <v>3</v>
+      </c>
+      <c r="F70" s="74" t="s">
+        <v>327</v>
+      </c>
+      <c r="I70" s="74" t="s">
+        <v>32</v>
+      </c>
+      <c r="L70" s="78" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="71" spans="1:14" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A71" s="74" t="s">
+        <v>332</v>
+      </c>
+      <c r="B71" s="75">
+        <v>9</v>
+      </c>
+      <c r="C71" s="78" t="s">
+        <v>326</v>
+      </c>
+      <c r="D71" s="74" t="s">
+        <v>320</v>
+      </c>
+      <c r="E71" s="75">
+        <v>12</v>
+      </c>
+      <c r="F71" s="74" t="s">
+        <v>328</v>
+      </c>
+      <c r="I71" s="74" t="s">
+        <v>32</v>
+      </c>
+      <c r="L71" s="78" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="72" spans="1:14" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A72" s="74" t="s">
+        <v>350</v>
+      </c>
+      <c r="B72" s="75">
         <v>1</v>
       </c>
-      <c r="F63" s="74" t="s">
+      <c r="C72" s="74" t="s">
+        <v>29</v>
+      </c>
+      <c r="D72" s="74" t="s">
+        <v>30</v>
+      </c>
+      <c r="E72" s="75">
+        <v>15</v>
+      </c>
+      <c r="F72" s="74" t="s">
+        <v>31</v>
+      </c>
+      <c r="G72" s="79">
+        <v>1</v>
+      </c>
+      <c r="I72" s="74" t="s">
+        <v>243</v>
+      </c>
+      <c r="N72" s="74" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="73" spans="1:14" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A73" s="74" t="s">
+        <v>350</v>
+      </c>
+      <c r="B73" s="75">
+        <v>2</v>
+      </c>
+      <c r="C73" s="74" t="s">
+        <v>33</v>
+      </c>
+      <c r="D73" s="74" t="s">
+        <v>30</v>
+      </c>
+      <c r="E73" s="75">
+        <v>25</v>
+      </c>
+      <c r="F73" s="74" t="s">
+        <v>34</v>
+      </c>
+      <c r="G73" s="79">
+        <v>2</v>
+      </c>
+      <c r="I73" s="74" t="s">
+        <v>243</v>
+      </c>
+      <c r="N73" s="74" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="74" spans="1:14" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A74" s="74" t="s">
+        <v>350</v>
+      </c>
+      <c r="B74" s="75">
+        <v>3</v>
+      </c>
+      <c r="C74" s="74" t="s">
+        <v>102</v>
+      </c>
+      <c r="D74" s="74" t="s">
+        <v>30</v>
+      </c>
+      <c r="E74" s="75">
+        <v>14</v>
+      </c>
+      <c r="F74" s="74" t="s">
+        <v>103</v>
+      </c>
+      <c r="I74" s="74" t="s">
+        <v>201</v>
+      </c>
+      <c r="N74" s="74" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="75" spans="1:14" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="74" t="s">
+        <v>350</v>
+      </c>
+      <c r="B75" s="75">
+        <v>4</v>
+      </c>
+      <c r="C75" s="74" t="s">
+        <v>100</v>
+      </c>
+      <c r="D75" s="74" t="s">
+        <v>36</v>
+      </c>
+      <c r="E75" s="75">
+        <v>8</v>
+      </c>
+      <c r="F75" s="74" t="s">
+        <v>101</v>
+      </c>
+      <c r="I75" s="74" t="s">
+        <v>202</v>
+      </c>
+      <c r="N75" s="74" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="76" spans="1:14" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A76" s="74" t="s">
+        <v>350</v>
+      </c>
+      <c r="B76" s="75">
+        <v>5</v>
+      </c>
+      <c r="C76" s="74" t="s">
+        <v>104</v>
+      </c>
+      <c r="D76" s="74" t="s">
+        <v>30</v>
+      </c>
+      <c r="E76" s="75">
+        <v>8</v>
+      </c>
+      <c r="F76" s="74" t="s">
+        <v>105</v>
+      </c>
+      <c r="I76" s="74" t="s">
+        <v>188</v>
+      </c>
+      <c r="L76" s="74" t="s">
+        <v>335</v>
+      </c>
+      <c r="N76" s="74" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="77" spans="1:14" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A77" s="74" t="s">
+        <v>350</v>
+      </c>
+      <c r="B77" s="75">
+        <v>6</v>
+      </c>
+      <c r="C77" s="74" t="s">
+        <v>106</v>
+      </c>
+      <c r="D77" s="74" t="s">
+        <v>30</v>
+      </c>
+      <c r="E77" s="75">
+        <v>61</v>
+      </c>
+      <c r="F77" s="74" t="s">
+        <v>107</v>
+      </c>
+      <c r="I77" s="74" t="s">
+        <v>188</v>
+      </c>
+      <c r="L77" s="74" t="s">
         <v>336</v>
       </c>
-      <c r="I63" s="74" t="s">
+      <c r="N77" s="74" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="78" spans="1:14" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A78" s="74" t="s">
+        <v>350</v>
+      </c>
+      <c r="B78" s="75">
+        <v>7</v>
+      </c>
+      <c r="C78" s="74" t="s">
+        <v>118</v>
+      </c>
+      <c r="D78" s="74" t="s">
+        <v>36</v>
+      </c>
+      <c r="E78" s="75">
+        <v>8</v>
+      </c>
+      <c r="F78" s="74" t="s">
+        <v>119</v>
+      </c>
+      <c r="I78" s="74" t="s">
         <v>32</v>
       </c>
-      <c r="L63" s="78" t="s">
-        <v>335</v>
-      </c>
-      <c r="M63" s="74" t="s">
-        <v>177</v>
+      <c r="L78" s="74" t="s">
+        <v>352</v>
+      </c>
+      <c r="N78" s="74" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="79" spans="1:14" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A79" s="74" t="s">
+        <v>350</v>
+      </c>
+      <c r="B79" s="75">
+        <v>8</v>
+      </c>
+      <c r="C79" s="78" t="s">
+        <v>120</v>
+      </c>
+      <c r="D79" s="74" t="s">
+        <v>30</v>
+      </c>
+      <c r="E79" s="75">
+        <v>12</v>
+      </c>
+      <c r="F79" s="74" t="s">
+        <v>142</v>
+      </c>
+      <c r="I79" s="74" t="s">
+        <v>354</v>
+      </c>
+      <c r="L79" s="78"/>
+      <c r="N79" s="74" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="80" spans="1:14" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A80" s="74" t="s">
+        <v>350</v>
+      </c>
+      <c r="B80" s="75">
+        <v>9</v>
+      </c>
+      <c r="C80" s="74" t="s">
+        <v>108</v>
+      </c>
+      <c r="D80" s="74" t="s">
+        <v>30</v>
+      </c>
+      <c r="E80" s="75">
+        <v>16</v>
+      </c>
+      <c r="F80" s="74" t="s">
+        <v>109</v>
+      </c>
+      <c r="I80" s="74" t="s">
+        <v>244</v>
+      </c>
+      <c r="N80" s="74" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="81" spans="1:14" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A81" s="74" t="s">
+        <v>350</v>
+      </c>
+      <c r="B81" s="75">
+        <v>10</v>
+      </c>
+      <c r="C81" s="74" t="s">
+        <v>110</v>
+      </c>
+      <c r="D81" s="74" t="s">
+        <v>36</v>
+      </c>
+      <c r="E81" s="75">
+        <v>8</v>
+      </c>
+      <c r="F81" s="74" t="s">
+        <v>111</v>
+      </c>
+      <c r="G81" s="79">
+        <v>4</v>
+      </c>
+      <c r="I81" s="74" t="s">
+        <v>283</v>
+      </c>
+      <c r="N81" s="74" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="82" spans="1:14" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A82" s="74" t="s">
+        <v>350</v>
+      </c>
+      <c r="B82" s="75">
+        <v>11</v>
+      </c>
+      <c r="C82" s="78" t="s">
+        <v>343</v>
+      </c>
+      <c r="D82" s="74" t="s">
+        <v>30</v>
+      </c>
+      <c r="E82" s="75">
+        <v>1</v>
+      </c>
+      <c r="F82" s="74" t="s">
+        <v>344</v>
+      </c>
+      <c r="I82" s="74" t="s">
+        <v>32</v>
+      </c>
+      <c r="L82" s="78" t="s">
+        <v>343</v>
+      </c>
+      <c r="M82" s="74" t="s">
+        <v>183</v>
       </c>
     </row>
   </sheetData>
@@ -4406,10 +4990,10 @@
         <v>17</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="E1" s="16" t="s">
         <v>16</v>
@@ -4433,7 +5017,7 @@
         <v>21</v>
       </c>
       <c r="L1" s="40" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="M1" s="16" t="s">
         <v>23</v>
@@ -4572,86 +5156,86 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="85" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="B2" s="86" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="C2" s="85" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="D2" s="87" t="s">
-        <v>214</v>
+        <v>220</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="88" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="B3" s="89" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="C3" s="89" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="D3" s="87" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="85" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="B4" s="86" t="s">
-        <v>193</v>
+        <v>199</v>
       </c>
       <c r="C4" s="85" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="D4" s="86" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="92" customFormat="1" ht="128.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="90" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="B5" s="91" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="C5" s="92" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="D5" s="91" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="92" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A6" s="90" t="s">
-        <v>197</v>
+        <v>203</v>
       </c>
       <c r="B6" s="91" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
       <c r="C6" s="92" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="D6" s="91" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="92" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A7" s="90" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="B7" s="91" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="C7" s="92" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="D7" s="91" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
     </row>
     <row r="8" spans="1:4" s="92" customFormat="1" ht="15" x14ac:dyDescent="0.2">
@@ -4661,422 +5245,422 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="85" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B9" s="86" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="C9" s="85" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="D9" s="86" t="s">
-        <v>232</v>
+        <v>238</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="85" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B10" s="86" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="C10" s="85" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="D10" s="86" t="s">
-        <v>233</v>
+        <v>239</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="94" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B11" s="86" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C11" s="85" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="D11" s="86" t="s">
-        <v>234</v>
+        <v>240</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="85" t="s">
-        <v>331</v>
+        <v>339</v>
       </c>
       <c r="B12" s="86" t="s">
-        <v>332</v>
+        <v>340</v>
       </c>
       <c r="C12" s="85" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="D12" s="86" t="s">
-        <v>333</v>
+        <v>341</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A13" s="85" t="s">
-        <v>311</v>
+        <v>318</v>
       </c>
       <c r="B13" s="86" t="s">
-        <v>314</v>
+        <v>321</v>
       </c>
       <c r="C13" s="85" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="D13" s="86" t="s">
-        <v>334</v>
+        <v>342</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="85" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B14" s="86" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C14" s="85" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="D14" s="86" t="s">
-        <v>234</v>
+        <v>240</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="85" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B15" s="86" t="s">
-        <v>290</v>
+        <v>297</v>
       </c>
       <c r="C15" s="85" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="D15" s="86" t="s">
-        <v>292</v>
+        <v>299</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="85" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B16" s="86" t="s">
-        <v>291</v>
+        <v>298</v>
       </c>
       <c r="C16" s="85" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="D16" s="86" t="s">
-        <v>293</v>
+        <v>300</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="85" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="B17" s="86" t="s">
-        <v>220</v>
+        <v>226</v>
       </c>
       <c r="C17" s="85" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="D17" s="86" t="s">
-        <v>229</v>
+        <v>235</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="85" t="s">
-        <v>219</v>
+        <v>225</v>
       </c>
       <c r="B18" s="86" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
       <c r="C18" s="85" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="D18" s="86" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="85" t="s">
-        <v>223</v>
+        <v>229</v>
       </c>
       <c r="B19" s="86" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
       <c r="C19" s="85" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="D19" s="86" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="85" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B20" s="86" t="s">
-        <v>222</v>
+        <v>228</v>
       </c>
       <c r="C20" s="85" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="D20" s="86" t="s">
-        <v>317</v>
+        <v>324</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="85" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B21" s="86" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="C21" s="85" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="D21" s="86" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="85" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B22" s="86" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
       <c r="C22" s="85" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="D22" s="86" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="85" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B23" s="86" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="C23" s="85" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="D23" s="86" t="s">
-        <v>186</v>
+        <v>192</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="85" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
       <c r="B24" s="86" t="s">
-        <v>205</v>
+        <v>211</v>
       </c>
       <c r="C24" s="85" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="D24" s="86" t="s">
-        <v>206</v>
+        <v>212</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="85" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="B25" s="86" t="s">
-        <v>207</v>
+        <v>213</v>
       </c>
       <c r="C25" s="85" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="D25" s="86" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="88" t="s">
-        <v>326</v>
+        <v>333</v>
       </c>
       <c r="B26" s="86" t="s">
-        <v>210</v>
+        <v>216</v>
       </c>
       <c r="C26" s="85" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="D26" s="86" t="s">
-        <v>211</v>
+        <v>217</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="85" t="s">
-        <v>327</v>
+        <v>334</v>
       </c>
       <c r="B27" s="86" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C27" s="85" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="D27" s="86" t="s">
-        <v>280</v>
+        <v>287</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="85" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B28" s="86" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C28" s="85" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="D28" s="86" t="s">
-        <v>281</v>
+        <v>288</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="85" t="s">
-        <v>328</v>
+        <v>335</v>
       </c>
       <c r="B29" s="86" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C29" s="85" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="D29" s="86" t="s">
-        <v>330</v>
+        <v>338</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="85" t="s">
-        <v>329</v>
+        <v>336</v>
       </c>
       <c r="B30" s="86" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C30" s="85" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="D30" s="86" t="s">
-        <v>341</v>
+        <v>349</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="88" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="B31" s="86" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="C31" s="85" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="D31" s="86" t="s">
-        <v>282</v>
+        <v>289</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="88" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="B32" s="86" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="C32" s="85" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="D32" s="86" t="s">
-        <v>283</v>
+        <v>290</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="88" t="s">
-        <v>287</v>
+        <v>294</v>
       </c>
       <c r="B33" s="86" t="s">
-        <v>288</v>
+        <v>295</v>
       </c>
       <c r="C33" s="85" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="D33" s="86" t="s">
-        <v>289</v>
+        <v>296</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="88" t="s">
-        <v>318</v>
+        <v>325</v>
       </c>
       <c r="B34" s="86" t="s">
-        <v>320</v>
+        <v>327</v>
       </c>
       <c r="C34" s="85" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="D34" s="86" t="s">
-        <v>337</v>
+        <v>345</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="85" t="s">
-        <v>319</v>
+        <v>326</v>
       </c>
       <c r="B35" s="86" t="s">
-        <v>321</v>
+        <v>328</v>
       </c>
       <c r="C35" s="85" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="D35" s="86" t="s">
-        <v>338</v>
+        <v>346</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="85" t="s">
-        <v>323</v>
+        <v>330</v>
       </c>
       <c r="B36" s="86" t="s">
-        <v>324</v>
+        <v>331</v>
       </c>
       <c r="C36" s="85" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="D36" s="86" t="s">
-        <v>339</v>
+        <v>347</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="85" t="s">
-        <v>335</v>
+        <v>343</v>
       </c>
       <c r="B37" s="86" t="s">
-        <v>336</v>
+        <v>344</v>
       </c>
       <c r="C37" s="85" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="D37" s="86" t="s">
-        <v>340</v>
+        <v>348</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="85" t="s">
-        <v>344</v>
+        <v>352</v>
       </c>
       <c r="B38" s="86" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="C38" s="85" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="D38" s="86" t="s">
-        <v>345</v>
+        <v>353</v>
       </c>
     </row>
   </sheetData>
@@ -5105,25 +5689,25 @@
   <sheetData>
     <row r="1" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="G1" s="11" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -5200,7 +5784,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="B1" s="51" t="s">
         <v>22</v>
@@ -5285,19 +5869,19 @@
         <v>79</v>
       </c>
       <c r="H1" s="10" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="I1" s="10" t="s">
-        <v>284</v>
+        <v>291</v>
       </c>
       <c r="J1" s="10" t="s">
-        <v>285</v>
+        <v>292</v>
       </c>
       <c r="K1" s="10"/>
     </row>
     <row r="2" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="32" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="B2" s="23">
         <v>1</v>
@@ -5306,7 +5890,7 @@
         <v>81</v>
       </c>
       <c r="D2" s="21" t="s">
-        <v>240</v>
+        <v>247</v>
       </c>
       <c r="E2" s="26" t="s">
         <v>36</v>
@@ -5314,7 +5898,7 @@
     </row>
     <row r="3" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="32" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="B3" s="23">
         <v>2</v>
@@ -5323,7 +5907,7 @@
         <v>80</v>
       </c>
       <c r="D3" s="21" t="s">
-        <v>241</v>
+        <v>248</v>
       </c>
       <c r="E3" s="26" t="s">
         <v>36</v>
@@ -5331,16 +5915,16 @@
     </row>
     <row r="4" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="32" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="B4" s="23">
         <v>3</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
       <c r="D4" s="21" t="s">
-        <v>242</v>
+        <v>249</v>
       </c>
       <c r="E4" s="26" t="s">
         <v>36</v>
@@ -5348,16 +5932,16 @@
     </row>
     <row r="5" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="32" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="B5" s="23">
         <v>4</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
       <c r="D5" s="21" t="s">
-        <v>243</v>
+        <v>250</v>
       </c>
       <c r="E5" s="26" t="s">
         <v>36</v>
@@ -5365,16 +5949,16 @@
     </row>
     <row r="6" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="32" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="B6" s="23">
         <v>5</v>
       </c>
       <c r="C6" s="20" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
       <c r="D6" s="21" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="E6" s="26" t="s">
         <v>36</v>
@@ -5382,7 +5966,7 @@
     </row>
     <row r="7" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="32" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="B7" s="23">
         <v>6</v>
@@ -5391,7 +5975,7 @@
         <v>74</v>
       </c>
       <c r="D7" s="21" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="E7" s="26" t="s">
         <v>36</v>
@@ -5399,7 +5983,7 @@
     </row>
     <row r="8" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="32" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="B8" s="23">
         <v>1</v>
@@ -5408,7 +5992,7 @@
         <v>74</v>
       </c>
       <c r="D8" s="21" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="E8" s="26" t="s">
         <v>36</v>
@@ -5416,7 +6000,7 @@
     </row>
     <row r="9" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="32" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="B9" s="23">
         <v>2</v>
@@ -5425,7 +6009,7 @@
         <v>81</v>
       </c>
       <c r="D9" s="19" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="E9" s="26" t="s">
         <v>36</v>
@@ -5433,7 +6017,7 @@
     </row>
     <row r="10" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="32" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="B10" s="23">
         <v>3</v>
@@ -5442,7 +6026,7 @@
         <v>80</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="E10" s="26" t="s">
         <v>36</v>
@@ -5450,7 +6034,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B11" s="23">
         <v>1</v>
@@ -5459,7 +6043,7 @@
         <v>74</v>
       </c>
       <c r="D11" s="65" t="s">
-        <v>244</v>
+        <v>251</v>
       </c>
       <c r="E11" t="s">
         <v>36</v>
@@ -5468,7 +6052,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B12" s="23">
         <v>2</v>
@@ -5486,7 +6070,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B13" s="23">
         <v>3</v>
@@ -5495,7 +6079,7 @@
         <v>81</v>
       </c>
       <c r="D13" s="25" t="s">
-        <v>301</v>
+        <v>308</v>
       </c>
       <c r="E13" t="s">
         <v>36</v>
@@ -5504,7 +6088,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B14" s="23">
         <v>4</v>
@@ -5513,7 +6097,7 @@
         <v>80</v>
       </c>
       <c r="D14" s="25" t="s">
-        <v>302</v>
+        <v>309</v>
       </c>
       <c r="E14" t="s">
         <v>36</v>
@@ -5522,16 +6106,16 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="64" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B15" s="66">
         <v>1</v>
       </c>
       <c r="C15" s="64" t="s">
-        <v>245</v>
+        <v>252</v>
       </c>
       <c r="D15" s="64" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E15" s="64" t="s">
         <v>30</v>
@@ -5540,16 +6124,16 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="64" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B16" s="66">
         <v>2</v>
       </c>
       <c r="C16" s="64" t="s">
-        <v>246</v>
+        <v>253</v>
       </c>
       <c r="D16" s="64" t="s">
-        <v>247</v>
+        <v>254</v>
       </c>
       <c r="E16" s="64" t="s">
         <v>30</v>
@@ -5558,16 +6142,16 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="64" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B17" s="66">
         <v>3</v>
       </c>
       <c r="C17" s="64" t="s">
-        <v>248</v>
+        <v>255</v>
       </c>
       <c r="D17" s="64" t="s">
-        <v>249</v>
+        <v>256</v>
       </c>
       <c r="E17" s="64" t="s">
         <v>30</v>
@@ -5576,16 +6160,16 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="64" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B18" s="66">
         <v>4</v>
       </c>
       <c r="C18" s="64" t="s">
-        <v>250</v>
+        <v>257</v>
       </c>
       <c r="D18" s="64" t="s">
-        <v>251</v>
+        <v>258</v>
       </c>
       <c r="E18" s="64" t="s">
         <v>30</v>
@@ -5594,16 +6178,16 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="64" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B19" s="66">
         <v>5</v>
       </c>
       <c r="C19" s="64" t="s">
-        <v>252</v>
+        <v>259</v>
       </c>
       <c r="D19" s="64" t="s">
-        <v>253</v>
+        <v>260</v>
       </c>
       <c r="E19" s="64" t="s">
         <v>30</v>
@@ -5612,16 +6196,16 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="64" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B20" s="66">
         <v>6</v>
       </c>
       <c r="C20" s="64" t="s">
-        <v>254</v>
+        <v>261</v>
       </c>
       <c r="D20" s="64" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
       <c r="E20" s="64" t="s">
         <v>30</v>
@@ -5630,16 +6214,16 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="64" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B21" s="66">
         <v>7</v>
       </c>
       <c r="C21" s="64" t="s">
-        <v>256</v>
+        <v>263</v>
       </c>
       <c r="D21" s="64" t="s">
-        <v>257</v>
+        <v>264</v>
       </c>
       <c r="E21" s="64" t="s">
         <v>30</v>
@@ -5647,16 +6231,16 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="64" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B22" s="66">
         <v>8</v>
       </c>
       <c r="C22" s="64" t="s">
-        <v>258</v>
+        <v>265</v>
       </c>
       <c r="D22" s="64" t="s">
-        <v>259</v>
+        <v>266</v>
       </c>
       <c r="E22" s="64" t="s">
         <v>30</v>
@@ -5664,16 +6248,16 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="64" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B23" s="66">
         <v>9</v>
       </c>
       <c r="C23" s="64" t="s">
-        <v>260</v>
+        <v>267</v>
       </c>
       <c r="D23" s="64" t="s">
-        <v>261</v>
+        <v>268</v>
       </c>
       <c r="E23" s="64" t="s">
         <v>30</v>
@@ -5681,16 +6265,16 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="64" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B24" s="66">
         <v>10</v>
       </c>
       <c r="C24" s="64" t="s">
-        <v>262</v>
+        <v>269</v>
       </c>
       <c r="D24" s="64" t="s">
-        <v>263</v>
+        <v>270</v>
       </c>
       <c r="E24" s="64" t="s">
         <v>30</v>
@@ -5698,16 +6282,16 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="64" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B25" s="66">
         <v>11</v>
       </c>
       <c r="C25" s="64" t="s">
-        <v>264</v>
+        <v>271</v>
       </c>
       <c r="D25" s="64" t="s">
-        <v>265</v>
+        <v>272</v>
       </c>
       <c r="E25" s="64" t="s">
         <v>30</v>
@@ -5715,16 +6299,16 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="64" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B26" s="66">
         <v>12</v>
       </c>
       <c r="C26" s="64" t="s">
-        <v>266</v>
+        <v>273</v>
       </c>
       <c r="D26" s="64" t="s">
-        <v>267</v>
+        <v>274</v>
       </c>
       <c r="E26" s="64" t="s">
         <v>30</v>
@@ -5732,16 +6316,16 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="64" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B27" s="66">
         <v>13</v>
       </c>
       <c r="C27" s="64" t="s">
-        <v>268</v>
+        <v>275</v>
       </c>
       <c r="D27" s="64" t="s">
-        <v>269</v>
+        <v>276</v>
       </c>
       <c r="E27" s="64" t="s">
         <v>30</v>
@@ -5749,16 +6333,16 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="64" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B28" s="66">
         <v>14</v>
       </c>
       <c r="C28" s="64" t="s">
-        <v>270</v>
+        <v>277</v>
       </c>
       <c r="D28" s="64" t="s">
-        <v>271</v>
+        <v>278</v>
       </c>
       <c r="E28" s="64" t="s">
         <v>30</v>
@@ -5766,16 +6350,16 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="64" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B29" s="66">
         <v>15</v>
       </c>
       <c r="C29" s="64" t="s">
-        <v>272</v>
+        <v>279</v>
       </c>
       <c r="D29" s="64" t="s">
-        <v>273</v>
+        <v>280</v>
       </c>
       <c r="E29" s="64" t="s">
         <v>30</v>
@@ -5783,16 +6367,16 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="64" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B30" s="66">
         <v>16</v>
       </c>
       <c r="C30" s="64" t="s">
-        <v>274</v>
+        <v>281</v>
       </c>
       <c r="D30" s="64" t="s">
-        <v>275</v>
+        <v>282</v>
       </c>
       <c r="E30" s="64" t="s">
         <v>30</v>
@@ -5800,16 +6384,16 @@
     </row>
     <row r="31" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="64" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B31" s="66">
         <v>1</v>
       </c>
       <c r="C31" s="64" t="s">
-        <v>277</v>
+        <v>284</v>
       </c>
       <c r="D31" s="64" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E31" s="26" t="s">
         <v>36</v>
@@ -5818,7 +6402,7 @@
     </row>
     <row r="32" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="64" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B32" s="66">
         <v>2</v>
@@ -5827,7 +6411,7 @@
         <v>1</v>
       </c>
       <c r="D32" s="64" t="s">
-        <v>247</v>
+        <v>254</v>
       </c>
       <c r="E32" s="26" t="s">
         <v>36</v>
@@ -5836,7 +6420,7 @@
     </row>
     <row r="33" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="64" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B33" s="66">
         <v>3</v>
@@ -5845,7 +6429,7 @@
         <v>2</v>
       </c>
       <c r="D33" s="64" t="s">
-        <v>249</v>
+        <v>256</v>
       </c>
       <c r="E33" s="26" t="s">
         <v>36</v>
@@ -5854,7 +6438,7 @@
     </row>
     <row r="34" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="64" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B34" s="66">
         <v>4</v>
@@ -5863,7 +6447,7 @@
         <v>3</v>
       </c>
       <c r="D34" s="64" t="s">
-        <v>251</v>
+        <v>258</v>
       </c>
       <c r="E34" s="26" t="s">
         <v>36</v>
@@ -5872,7 +6456,7 @@
     </row>
     <row r="35" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="64" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B35" s="66">
         <v>5</v>
@@ -5881,7 +6465,7 @@
         <v>4</v>
       </c>
       <c r="D35" s="64" t="s">
-        <v>253</v>
+        <v>260</v>
       </c>
       <c r="E35" s="26" t="s">
         <v>36</v>
@@ -5890,7 +6474,7 @@
     </row>
     <row r="36" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="64" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B36" s="66">
         <v>6</v>
@@ -5899,7 +6483,7 @@
         <v>5</v>
       </c>
       <c r="D36" s="64" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
       <c r="E36" s="26" t="s">
         <v>36</v>
@@ -5908,7 +6492,7 @@
     </row>
     <row r="37" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" s="64" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B37" s="66">
         <v>7</v>
@@ -5917,7 +6501,7 @@
         <v>6</v>
       </c>
       <c r="D37" s="64" t="s">
-        <v>257</v>
+        <v>264</v>
       </c>
       <c r="E37" s="26" t="s">
         <v>36</v>
@@ -5925,7 +6509,7 @@
     </row>
     <row r="38" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" s="64" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B38" s="66">
         <v>8</v>
@@ -5934,7 +6518,7 @@
         <v>7</v>
       </c>
       <c r="D38" s="64" t="s">
-        <v>259</v>
+        <v>266</v>
       </c>
       <c r="E38" s="26" t="s">
         <v>36</v>
@@ -5942,7 +6526,7 @@
     </row>
     <row r="39" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A39" s="64" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B39" s="66">
         <v>9</v>
@@ -5951,7 +6535,7 @@
         <v>8</v>
       </c>
       <c r="D39" s="64" t="s">
-        <v>261</v>
+        <v>268</v>
       </c>
       <c r="E39" s="26" t="s">
         <v>36</v>
@@ -5959,7 +6543,7 @@
     </row>
     <row r="40" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A40" s="64" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B40" s="66">
         <v>10</v>
@@ -5968,7 +6552,7 @@
         <v>9</v>
       </c>
       <c r="D40" s="64" t="s">
-        <v>263</v>
+        <v>270</v>
       </c>
       <c r="E40" s="26" t="s">
         <v>36</v>
@@ -5976,7 +6560,7 @@
     </row>
     <row r="41" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A41" s="64" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B41" s="66">
         <v>11</v>
@@ -5985,7 +6569,7 @@
         <v>10</v>
       </c>
       <c r="D41" s="64" t="s">
-        <v>265</v>
+        <v>272</v>
       </c>
       <c r="E41" s="26" t="s">
         <v>36</v>
@@ -5993,7 +6577,7 @@
     </row>
     <row r="42" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" s="64" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B42" s="66">
         <v>12</v>
@@ -6002,7 +6586,7 @@
         <v>11</v>
       </c>
       <c r="D42" s="64" t="s">
-        <v>267</v>
+        <v>274</v>
       </c>
       <c r="E42" s="26" t="s">
         <v>36</v>
@@ -6010,7 +6594,7 @@
     </row>
     <row r="43" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A43" s="64" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B43" s="66">
         <v>13</v>
@@ -6019,7 +6603,7 @@
         <v>12</v>
       </c>
       <c r="D43" s="64" t="s">
-        <v>269</v>
+        <v>276</v>
       </c>
       <c r="E43" s="26" t="s">
         <v>36</v>
@@ -6027,7 +6611,7 @@
     </row>
     <row r="44" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A44" s="64" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B44" s="66">
         <v>14</v>
@@ -6036,7 +6620,7 @@
         <v>13</v>
       </c>
       <c r="D44" s="64" t="s">
-        <v>271</v>
+        <v>278</v>
       </c>
       <c r="E44" s="26" t="s">
         <v>36</v>
@@ -6044,16 +6628,16 @@
     </row>
     <row r="45" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A45" s="64" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B45" s="66">
         <v>15</v>
       </c>
       <c r="C45" s="64" t="s">
-        <v>286</v>
+        <v>293</v>
       </c>
       <c r="D45" s="64" t="s">
-        <v>273</v>
+        <v>280</v>
       </c>
       <c r="E45" s="26" t="s">
         <v>36</v>
@@ -6061,16 +6645,16 @@
     </row>
     <row r="46" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A46" s="64" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B46" s="66">
         <v>16</v>
       </c>
       <c r="C46" s="64" t="s">
-        <v>278</v>
+        <v>285</v>
       </c>
       <c r="D46" s="64" t="s">
-        <v>275</v>
+        <v>282</v>
       </c>
       <c r="E46" s="26" t="s">
         <v>36</v>
@@ -6078,7 +6662,7 @@
     </row>
     <row r="47" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A47" s="26" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B47" s="23">
         <v>1</v>
@@ -6096,7 +6680,7 @@
     </row>
     <row r="48" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A48" s="26" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B48" s="23">
         <v>2</v>
@@ -6105,7 +6689,7 @@
         <v>74</v>
       </c>
       <c r="D48" s="26" t="s">
-        <v>244</v>
+        <v>251</v>
       </c>
       <c r="E48" s="26" t="s">
         <v>36</v>
@@ -6114,7 +6698,7 @@
     </row>
     <row r="49" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A49" s="26" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B49" s="23">
         <v>3</v>
@@ -6123,7 +6707,7 @@
         <v>81</v>
       </c>
       <c r="D49" s="26" t="s">
-        <v>301</v>
+        <v>308</v>
       </c>
       <c r="E49" s="26" t="s">
         <v>36</v>
@@ -6132,7 +6716,7 @@
     </row>
     <row r="50" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A50" s="26" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B50" s="23">
         <v>4</v>
@@ -6141,7 +6725,7 @@
         <v>80</v>
       </c>
       <c r="D50" s="26" t="s">
-        <v>302</v>
+        <v>309</v>
       </c>
       <c r="E50" s="26" t="s">
         <v>36</v>
@@ -6150,7 +6734,7 @@
     </row>
     <row r="51" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A51" s="32" t="s">
-        <v>322</v>
+        <v>329</v>
       </c>
       <c r="C51" s="31" t="s">
         <v>83</v>
@@ -6167,7 +6751,7 @@
     </row>
     <row r="52" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A52" s="32" t="s">
-        <v>322</v>
+        <v>329</v>
       </c>
       <c r="C52" s="31" t="s">
         <v>74</v>
@@ -6182,13 +6766,13 @@
     </row>
     <row r="53" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A53" s="26" t="s">
-        <v>306</v>
+        <v>313</v>
       </c>
       <c r="C53" s="31" t="s">
-        <v>307</v>
+        <v>314</v>
       </c>
       <c r="D53" s="26" t="s">
-        <v>308</v>
+        <v>315</v>
       </c>
       <c r="E53" s="26" t="s">
         <v>30</v>
@@ -6196,13 +6780,13 @@
     </row>
     <row r="54" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A54" s="26" t="s">
-        <v>306</v>
+        <v>313</v>
       </c>
       <c r="C54" s="31" t="s">
-        <v>309</v>
+        <v>316</v>
       </c>
       <c r="D54" s="26" t="s">
-        <v>310</v>
+        <v>317</v>
       </c>
       <c r="E54" s="26" t="s">
         <v>30</v>
@@ -6239,46 +6823,46 @@
   <sheetData>
     <row r="1" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="44" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="B1" s="45" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="C1" s="45" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="D1" s="45" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="E1" s="45" t="s">
         <v>12</v>
       </c>
       <c r="F1" s="45" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="G1" s="45" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="H1" s="45" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="I1" s="45" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="J1" s="45" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="K1" s="45" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
       <c r="L1" s="45" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
       <c r="M1" s="45" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="N1" s="45" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>